<commit_message>
feature: finger update: data
</commit_message>
<xml_diff>
--- a/data/achievement.xlsx
+++ b/data/achievement.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\home\vick\dev\motleycrowd\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\home\vick\dev\motleycrowd-service\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66073D8-DF10-4E4D-B925-CE3F22495F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6A537E-D5D4-4661-8746-19201476AB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -818,7 +818,46 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>累计获得</t>
+      <t>月入过万</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>土块</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>与众不同</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>拥有</t>
     </r>
     <r>
       <rPr>
@@ -827,43 +866,43 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>1000</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>金币</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>月入过万</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>累计获得</t>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>个头衔</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>刻耳柏洛斯</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>拥有</t>
     </r>
     <r>
       <rPr>
@@ -872,43 +911,43 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>10000</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>金币</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>土块</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>累计获得</t>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>个头衔</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>知名人士</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>拥有</t>
     </r>
     <r>
       <rPr>
@@ -917,30 +956,30 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>100000</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>金币</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>与众不同</t>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>个头衔</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>低调</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -962,7 +1001,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>1</t>
+      <t>30</t>
     </r>
     <r>
       <rPr>
@@ -973,19 +1012,6 @@
         <charset val="134"/>
       </rPr>
       <t>个头衔</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>刻耳柏洛斯</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1017,20 +1043,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>个头衔</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>知名人士</t>
+      <t>个名片背景</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1062,20 +1075,20 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>个头衔</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>低调</t>
+      <t>个名片背景</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>选择困难症</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1107,51 +1120,6 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>个头衔</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>三原色</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>拥有</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
       <t>个名片背景</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1165,129 +1133,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>五彩斑斓的黑</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>拥有</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>个名片背景</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>选择困难症</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>拥有</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>30</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>个名片背景</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
       <t>社交达人</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>拥有</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>100</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>个名片背景</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2827,10 +2673,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{count: record.c.m0}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>category</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2935,6 +2777,148 @@
   </si>
   <si>
     <t>$asset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三原色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>身份证明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拥有1个名片背景</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>累计获得</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>银</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>币</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{count: record.c.m1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>累计获得</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>10000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>银</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>币</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>累计获得</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>100000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>银</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>币</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2942,7 +2926,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3013,6 +2997,27 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -3073,7 +3078,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3273,6 +3278,24 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3563,10 +3586,10 @@
   <dimension ref="A1:J175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F63" sqref="F63"/>
+      <selection pane="bottomRight" activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3604,48 +3627,48 @@
         <v>34</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>35</v>
       </c>
       <c r="I1" s="44" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="J1" s="44" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="55" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="55" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="55" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="G2" s="56" t="s">
+        <v>216</v>
+      </c>
+      <c r="H2" s="56" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="I2" s="54" t="s">
         <v>154</v>
       </c>
-      <c r="C2" s="56" t="s">
-        <v>155</v>
-      </c>
-      <c r="D2" s="55" t="s">
-        <v>156</v>
-      </c>
-      <c r="E2" s="55" t="s">
-        <v>157</v>
-      </c>
-      <c r="F2" s="57" t="s">
-        <v>158</v>
-      </c>
-      <c r="G2" s="56" t="s">
-        <v>223</v>
-      </c>
-      <c r="H2" s="56" t="s">
-        <v>159</v>
-      </c>
-      <c r="I2" s="54" t="s">
-        <v>160</v>
-      </c>
       <c r="J2" s="54" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
@@ -3665,16 +3688,16 @@
         <v>0</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="I3" s="45" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="J3" s="45" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -3695,16 +3718,16 @@
       </c>
       <c r="F4" s="37"/>
       <c r="G4" s="13" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I4" s="46" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="J4" s="46" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
@@ -3724,16 +3747,16 @@
         <v>0</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I5" s="45" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="J5" s="45" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -3756,16 +3779,16 @@
         <v>6</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I6" s="46" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="J6" s="46" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="9" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -3788,16 +3811,16 @@
         <v>7</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I7" s="47" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="J7" s="47" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
@@ -3817,16 +3840,16 @@
         <v>0</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I8" s="45" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="J8" s="45" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="9" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -3849,16 +3872,16 @@
         <v>8</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I9" s="47" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="J9" s="47" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -3881,16 +3904,16 @@
         <v>9</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I10" s="48" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="J10" s="48" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -3913,16 +3936,16 @@
         <v>10</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I11" s="46" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="J11" s="46" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
@@ -3945,16 +3968,16 @@
         <v>11</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I12" s="45" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="J12" s="45" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -3977,16 +4000,16 @@
         <v>12</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I13" s="48" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="J13" s="48" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="9" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -4009,16 +4032,16 @@
         <v>13</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I14" s="47" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="J14" s="47" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="20" customFormat="1" ht="62" x14ac:dyDescent="0.3">
@@ -4026,10 +4049,10 @@
         <v>113</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D15" s="20">
         <v>0</v>
@@ -4039,16 +4062,16 @@
       </c>
       <c r="F15" s="40"/>
       <c r="G15" s="22" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="I15" s="59" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="J15" s="59" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="23" customFormat="1" ht="62" x14ac:dyDescent="0.3">
@@ -4056,10 +4079,10 @@
         <v>114</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D16" s="23">
         <v>1</v>
@@ -4071,16 +4094,16 @@
         <v>14</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="I16" s="58" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="J16" s="58" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="9" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -4103,16 +4126,16 @@
         <v>15</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I17" s="47" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="J17" s="47" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="20" customFormat="1" ht="62" x14ac:dyDescent="0.3">
@@ -4120,10 +4143,10 @@
         <v>116</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D18" s="20">
         <v>0</v>
@@ -4133,16 +4156,16 @@
       </c>
       <c r="F18" s="40"/>
       <c r="G18" s="22" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="H18" s="22" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="I18" s="59" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="J18" s="59" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="20" customFormat="1" ht="62" x14ac:dyDescent="0.3">
@@ -4150,10 +4173,10 @@
         <v>117</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D19" s="20">
         <v>0</v>
@@ -4163,16 +4186,16 @@
       </c>
       <c r="F19" s="40"/>
       <c r="G19" s="22" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H19" s="22" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="I19" s="59" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J19" s="59" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="23" customFormat="1" ht="77.5" x14ac:dyDescent="0.3">
@@ -4180,10 +4203,10 @@
         <v>118</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D20" s="23">
         <v>1</v>
@@ -4195,16 +4218,16 @@
         <v>16</v>
       </c>
       <c r="G20" s="25" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="I20" s="58" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="J20" s="58" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="26" customFormat="1" ht="77.5" x14ac:dyDescent="0.3">
@@ -4212,10 +4235,10 @@
         <v>119</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D21" s="26">
         <v>2</v>
@@ -4227,16 +4250,16 @@
         <v>17</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H21" s="28" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="I21" s="60" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="J21" s="60" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="62" x14ac:dyDescent="0.3">
@@ -4256,16 +4279,16 @@
         <v>0</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="I22" s="61" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="J22" s="61" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="20" customFormat="1" ht="77.5" x14ac:dyDescent="0.3">
@@ -4273,10 +4296,10 @@
         <v>121</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D23" s="20">
         <v>0</v>
@@ -4286,16 +4309,16 @@
       </c>
       <c r="F23" s="40"/>
       <c r="G23" s="22" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H23" s="22" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="I23" s="59" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="J23" s="59" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="23" customFormat="1" ht="77.5" x14ac:dyDescent="0.3">
@@ -4303,10 +4326,10 @@
         <v>122</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D24" s="23">
         <v>1</v>
@@ -4318,16 +4341,16 @@
         <v>18</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="I24" s="58" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="J24" s="58" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="23" customFormat="1" ht="201.5" x14ac:dyDescent="0.3">
@@ -4335,10 +4358,10 @@
         <v>123</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D25" s="23">
         <v>1</v>
@@ -4348,16 +4371,16 @@
       </c>
       <c r="F25" s="41"/>
       <c r="G25" s="25" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H25" s="25" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="I25" s="58" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="J25" s="58" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="20" customFormat="1" ht="77.5" x14ac:dyDescent="0.3">
@@ -4365,10 +4388,10 @@
         <v>124</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D26" s="20">
         <v>0</v>
@@ -4378,16 +4401,16 @@
       </c>
       <c r="F26" s="40"/>
       <c r="G26" s="22" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H26" s="22" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="I26" s="59" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="J26" s="59" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="20" customFormat="1" ht="77.5" x14ac:dyDescent="0.3">
@@ -4395,10 +4418,10 @@
         <v>125</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D27" s="20">
         <v>0</v>
@@ -4408,16 +4431,16 @@
       </c>
       <c r="F27" s="40"/>
       <c r="G27" s="22" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H27" s="22" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="I27" s="59" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="J27" s="59" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="20" customFormat="1" ht="77.5" x14ac:dyDescent="0.3">
@@ -4425,10 +4448,10 @@
         <v>126</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D28" s="20">
         <v>0</v>
@@ -4438,16 +4461,16 @@
       </c>
       <c r="F28" s="40"/>
       <c r="G28" s="22" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H28" s="22" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="I28" s="59" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="J28" s="59" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="20" customFormat="1" ht="77.5" x14ac:dyDescent="0.3">
@@ -4455,10 +4478,10 @@
         <v>127</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D29" s="20">
         <v>0</v>
@@ -4468,16 +4491,16 @@
       </c>
       <c r="F29" s="40"/>
       <c r="G29" s="22" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="I29" s="59" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="J29" s="59" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="20" customFormat="1" ht="77.5" x14ac:dyDescent="0.3">
@@ -4485,10 +4508,10 @@
         <v>128</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C30" s="33" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D30" s="20">
         <v>0</v>
@@ -4498,16 +4521,16 @@
       </c>
       <c r="F30" s="40"/>
       <c r="G30" s="22" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="H30" s="22" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="I30" s="59" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="J30" s="59" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="20" customFormat="1" ht="201.5" x14ac:dyDescent="0.3">
@@ -4515,10 +4538,10 @@
         <v>129</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D31" s="20">
         <v>0</v>
@@ -4528,16 +4551,16 @@
       </c>
       <c r="F31" s="40"/>
       <c r="G31" s="22" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="H31" s="22" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="I31" s="59" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="J31" s="59" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
@@ -4547,8 +4570,8 @@
       <c r="B32" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="19" t="s">
-        <v>65</v>
+      <c r="C32" s="73" t="s">
+        <v>238</v>
       </c>
       <c r="D32" s="2">
         <v>0</v>
@@ -4557,16 +4580,16 @@
         <v>0</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I32" s="45" t="s">
-        <v>213</v>
+        <v>239</v>
       </c>
       <c r="J32" s="45" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -4574,10 +4597,10 @@
         <v>131</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="C33" s="70" t="s">
+        <v>240</v>
       </c>
       <c r="D33" s="5">
         <v>1</v>
@@ -4587,16 +4610,16 @@
       </c>
       <c r="F33" s="37"/>
       <c r="G33" s="13" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I33" s="46" t="s">
-        <v>213</v>
+        <v>239</v>
       </c>
       <c r="J33" s="46" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="9" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -4604,10 +4627,10 @@
         <v>132</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
+      </c>
+      <c r="C34" s="71" t="s">
+        <v>241</v>
       </c>
       <c r="D34" s="9">
         <v>2</v>
@@ -4619,16 +4642,16 @@
         <v>19</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H34" s="14" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I34" s="47" t="s">
-        <v>213</v>
+        <v>239</v>
       </c>
       <c r="J34" s="47" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
@@ -4636,10 +4659,10 @@
         <v>133</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D35" s="2">
         <v>0</v>
@@ -4648,16 +4671,16 @@
         <v>0</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="H35" s="12" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="I35" s="45" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="J35" s="45" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="1:10" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -4665,10 +4688,10 @@
         <v>134</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D36" s="5">
         <v>1</v>
@@ -4678,16 +4701,16 @@
       </c>
       <c r="F36" s="37"/>
       <c r="G36" s="13" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I36" s="46" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="J36" s="46" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="37" spans="1:10" s="9" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -4695,10 +4718,10 @@
         <v>135</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D37" s="9">
         <v>2</v>
@@ -4708,16 +4731,16 @@
       </c>
       <c r="F37" s="38"/>
       <c r="G37" s="14" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I37" s="47" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="J37" s="47" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="38" spans="1:10" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -4725,10 +4748,10 @@
         <v>136</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D38" s="7">
         <v>3</v>
@@ -4740,27 +4763,27 @@
         <v>20</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I38" s="48" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="J38" s="48" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>137</v>
       </c>
-      <c r="B39" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>79</v>
+      <c r="B39" s="68" t="s">
+        <v>236</v>
+      </c>
+      <c r="C39" s="68" t="s">
+        <v>237</v>
       </c>
       <c r="D39" s="2">
         <v>0</v>
@@ -4769,27 +4792,27 @@
         <v>0</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I39" s="45" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="J39" s="45" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="40" spans="1:10" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>138</v>
       </c>
-      <c r="B40" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>81</v>
+      <c r="B40" s="69" t="s">
+        <v>235</v>
+      </c>
+      <c r="C40" s="70" t="s">
+        <v>75</v>
       </c>
       <c r="D40" s="5">
         <v>1</v>
@@ -4799,16 +4822,16 @@
       </c>
       <c r="F40" s="37"/>
       <c r="G40" s="13" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I40" s="46" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="J40" s="46" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="41" spans="1:10" s="9" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -4816,10 +4839,10 @@
         <v>139</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>83</v>
+        <v>77</v>
+      </c>
+      <c r="C41" s="71" t="s">
+        <v>76</v>
       </c>
       <c r="D41" s="9">
         <v>2</v>
@@ -4829,16 +4852,16 @@
       </c>
       <c r="F41" s="38"/>
       <c r="G41" s="14" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I41" s="47" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="J41" s="47" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="42" spans="1:10" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -4846,10 +4869,10 @@
         <v>140</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>85</v>
+        <v>79</v>
+      </c>
+      <c r="C42" s="72" t="s">
+        <v>78</v>
       </c>
       <c r="D42" s="7">
         <v>3</v>
@@ -4861,16 +4884,16 @@
         <v>30</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I42" s="48" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="J42" s="48" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="62" x14ac:dyDescent="0.3">
@@ -4878,10 +4901,10 @@
         <v>141</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D43" s="5">
         <v>1</v>
@@ -4891,16 +4914,16 @@
       </c>
       <c r="F43" s="37"/>
       <c r="G43" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="H43" s="13" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="I43" s="62" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="J43" s="62" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="44" spans="1:10" s="9" customFormat="1" ht="62" x14ac:dyDescent="0.3">
@@ -4908,10 +4931,10 @@
         <v>142</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D44" s="9">
         <v>2</v>
@@ -4923,16 +4946,16 @@
         <v>21</v>
       </c>
       <c r="G44" s="14" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="I44" s="63" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="J44" s="63" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="45" spans="1:10" s="7" customFormat="1" ht="62" x14ac:dyDescent="0.3">
@@ -4940,10 +4963,10 @@
         <v>143</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D45" s="7">
         <v>3</v>
@@ -4955,16 +4978,16 @@
         <v>22</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="I45" s="64" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="J45" s="64" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:10" s="5" customFormat="1" ht="62" x14ac:dyDescent="0.3">
@@ -4972,10 +4995,10 @@
         <v>144</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D46" s="5">
         <v>1</v>
@@ -4985,16 +5008,16 @@
       </c>
       <c r="F46" s="37"/>
       <c r="G46" s="13" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="H46" s="13" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="I46" s="62" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="J46" s="62" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:10" s="9" customFormat="1" ht="62" x14ac:dyDescent="0.3">
@@ -5002,10 +5025,10 @@
         <v>145</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D47" s="9">
         <v>2</v>
@@ -5017,16 +5040,16 @@
         <v>23</v>
       </c>
       <c r="G47" s="14" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="H47" s="14" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="I47" s="63" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="J47" s="63" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="48" spans="1:10" s="7" customFormat="1" ht="62" x14ac:dyDescent="0.3">
@@ -5034,10 +5057,10 @@
         <v>146</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D48" s="7">
         <v>3</v>
@@ -5049,16 +5072,16 @@
         <v>24</v>
       </c>
       <c r="G48" s="15" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="I48" s="64" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="J48" s="64" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="49" spans="1:10" s="5" customFormat="1" ht="62" x14ac:dyDescent="0.3">
@@ -5066,10 +5089,10 @@
         <v>147</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D49" s="5">
         <v>1</v>
@@ -5081,16 +5104,16 @@
         <v>31</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="H49" s="13" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="I49" s="62" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="J49" s="62" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="9" customFormat="1" ht="62" x14ac:dyDescent="0.3">
@@ -5098,10 +5121,10 @@
         <v>148</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D50" s="9">
         <v>2</v>
@@ -5113,16 +5136,16 @@
         <v>32</v>
       </c>
       <c r="G50" s="14" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="I50" s="63" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="J50" s="63" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="51" spans="1:10" s="7" customFormat="1" ht="62" x14ac:dyDescent="0.3">
@@ -5130,10 +5153,10 @@
         <v>149</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D51" s="7">
         <v>3</v>
@@ -5145,16 +5168,16 @@
         <v>33</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="I51" s="64" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="J51" s="64" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="52" spans="1:10" s="23" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -5165,7 +5188,7 @@
         <v>5</v>
       </c>
       <c r="C52" s="29" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D52" s="23">
         <v>1</v>
@@ -5175,16 +5198,16 @@
       </c>
       <c r="F52" s="41"/>
       <c r="G52" s="25" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H52" s="25" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I52" s="49" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="J52" s="49" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="53" spans="1:10" s="23" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -5192,10 +5215,10 @@
         <v>151</v>
       </c>
       <c r="B53" s="29" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C53" s="29" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D53" s="23">
         <v>1</v>
@@ -5207,16 +5230,16 @@
         <v>25</v>
       </c>
       <c r="G53" s="25" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H53" s="25" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I53" s="49" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="J53" s="49" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
@@ -5224,10 +5247,10 @@
         <v>152</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D54" s="2">
         <v>0</v>
@@ -5236,16 +5259,16 @@
         <v>0</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H54" s="12" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I54" s="45" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="J54" s="45" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -5253,10 +5276,10 @@
         <v>153</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D55" s="5">
         <v>1</v>
@@ -5268,16 +5291,16 @@
         <v>26</v>
       </c>
       <c r="G55" s="13" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H55" s="13" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I55" s="46" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="J55" s="46" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="9" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -5285,10 +5308,10 @@
         <v>154</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D56" s="10">
         <v>2</v>
@@ -5300,16 +5323,16 @@
         <v>27</v>
       </c>
       <c r="G56" s="16" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H56" s="16" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I56" s="50" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="J56" s="47" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="57" spans="1:10" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -5317,10 +5340,10 @@
         <v>155</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D57" s="8">
         <v>3</v>
@@ -5332,16 +5355,16 @@
         <v>28</v>
       </c>
       <c r="G57" s="17" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H57" s="17" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I57" s="51" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="J57" s="48" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="23" customFormat="1" ht="139.5" x14ac:dyDescent="0.3">
@@ -5349,10 +5372,10 @@
         <v>156</v>
       </c>
       <c r="B58" s="29" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C58" s="29" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D58" s="24">
         <v>0</v>
@@ -5362,16 +5385,16 @@
       </c>
       <c r="F58" s="41"/>
       <c r="G58" s="29" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H58" s="29" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="I58" s="65" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="J58" s="58" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="59" spans="1:10" s="30" customFormat="1" ht="139.5" x14ac:dyDescent="0.3">
@@ -5379,10 +5402,10 @@
         <v>157</v>
       </c>
       <c r="B59" s="32" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C59" s="32" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D59" s="31">
         <v>1</v>
@@ -5394,16 +5417,16 @@
         <v>29</v>
       </c>
       <c r="G59" s="32" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H59" s="32" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="I59" s="66" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="J59" s="67" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>